<commit_message>
Added Run Mode concept
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/MasterSheet_B8.xlsx
+++ b/src/test/resources/testData/MasterSheet_B8.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23929"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ACB9901-5C4F-4D3B-BCA2-5280DAD564A5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="TestData" sheetId="1" r:id="rId1"/>
-    <sheet name="NewSheet" sheetId="2" r:id="rId2"/>
+    <sheet name="Test_Cases" sheetId="3" r:id="rId1"/>
+    <sheet name="TestData" sheetId="1" r:id="rId2"/>
+    <sheet name="NewSheet" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="61">
   <si>
     <t>Sr.No</t>
   </si>
@@ -180,12 +182,30 @@
   </si>
   <si>
     <t>pqr</t>
+  </si>
+  <si>
+    <t>TestCaseName</t>
+  </si>
+  <si>
+    <t>Run_Mode</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>TC04_Create_an_Account4</t>
+  </si>
+  <si>
+    <t>TC05_Create_an_Account5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -266,7 +286,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -278,6 +298,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -375,6 +398,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -410,6 +450,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -585,43 +642,129 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5150C5D-A284-42B7-845C-2E59D3FC34EB}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="5.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="16.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="9.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="9.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="8.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="9.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="9.36328125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.21875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.36328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A1" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
       <c r="J1" s="2"/>
       <c r="K1" s="8"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>35</v>
       </c>
@@ -662,7 +805,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -703,22 +846,22 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5" s="9" t="s">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A5" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
       <c r="J5" s="2"/>
       <c r="K5" s="8"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>35</v>
       </c>
@@ -759,7 +902,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>1</v>
       </c>
@@ -800,22 +943,22 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A9" s="9" t="s">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A9" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
       <c r="J9" s="2"/>
       <c r="K9" s="8"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>35</v>
       </c>
@@ -856,7 +999,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>1</v>
       </c>
@@ -904,39 +1047,39 @@
     <mergeCell ref="A9:I9"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="J3" r:id="rId1"/>
-    <hyperlink ref="J7" r:id="rId2"/>
-    <hyperlink ref="J11" r:id="rId3"/>
+    <hyperlink ref="J3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="J7" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="J11" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="5.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="5.36328125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="9.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="9.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="9.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="9.36328125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>34</v>
       </c>
       <c r="B1" s="6"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -959,7 +1102,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -982,7 +1125,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1005,7 +1148,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1028,7 +1171,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1051,7 +1194,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1074,7 +1217,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1097,7 +1240,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>7</v>
       </c>

</xml_diff>

<commit_message>
Updated screenshot path for Jenkins
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/MasterSheet_B8.xlsx
+++ b/src/test/resources/testData/MasterSheet_B8.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24026"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ACB9901-5C4F-4D3B-BCA2-5280DAD564A5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4603B28-4EAD-40FE-A9E2-4F5D06108260}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -646,7 +646,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>